<commit_message>
Almost finished printing neatly 1
</commit_message>
<xml_diff>
--- a/Project_Planning.xlsx
+++ b/Project_Planning.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3525" yWindow="0" windowWidth="27630" windowHeight="13020"/>
+    <workbookView xWindow="4695" yWindow="0" windowWidth="27630" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="To List" sheetId="1" r:id="rId1"/>
+    <sheet name="Printing neatly example" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>Task</t>
   </si>
@@ -87,13 +88,49 @@
   </si>
   <si>
     <t xml:space="preserve">Text Pre-processing </t>
+  </si>
+  <si>
+    <t>This</t>
+  </si>
+  <si>
+    <t>is</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>for</t>
+  </si>
+  <si>
+    <t>printing</t>
+  </si>
+  <si>
+    <t>neatly</t>
+  </si>
+  <si>
+    <t>Cost matrix</t>
+  </si>
+  <si>
+    <t>cost</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>i</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +146,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -118,7 +161,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -251,11 +294,106 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -271,6 +409,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,7 +717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -921,4 +1085,456 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:K21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="3.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="26">
+        <v>0</v>
+      </c>
+      <c r="E5" s="26">
+        <v>1</v>
+      </c>
+      <c r="F5" s="26">
+        <v>2</v>
+      </c>
+      <c r="G5" s="26">
+        <v>3</v>
+      </c>
+      <c r="H5" s="26">
+        <v>4</v>
+      </c>
+      <c r="I5" s="26">
+        <v>5</v>
+      </c>
+      <c r="J5" s="26">
+        <v>6</v>
+      </c>
+      <c r="K5" s="26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="23"/>
+      <c r="D6" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="26">
+        <v>0</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="15">
+        <v>1728</v>
+      </c>
+      <c r="E7" s="16">
+        <v>729</v>
+      </c>
+      <c r="F7" s="16">
+        <v>343</v>
+      </c>
+      <c r="G7" s="16">
+        <v>8</v>
+      </c>
+      <c r="H7" s="16">
+        <v>10000</v>
+      </c>
+      <c r="I7" s="16">
+        <v>10000</v>
+      </c>
+      <c r="J7" s="16">
+        <v>10000</v>
+      </c>
+      <c r="K7" s="17">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="26">
+        <v>1</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="18">
+        <v>10000</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2744</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1728</v>
+      </c>
+      <c r="G8" s="2">
+        <v>343</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0</v>
+      </c>
+      <c r="I8" s="2">
+        <v>10000</v>
+      </c>
+      <c r="J8" s="2">
+        <v>10000</v>
+      </c>
+      <c r="K8" s="19">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="26">
+        <v>2</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="18">
+        <v>10000</v>
+      </c>
+      <c r="E9" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3375</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1000</v>
+      </c>
+      <c r="H9" s="2">
+        <v>27</v>
+      </c>
+      <c r="I9" s="2">
+        <v>10000</v>
+      </c>
+      <c r="J9" s="2">
+        <v>10000</v>
+      </c>
+      <c r="K9" s="19">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="26">
+        <v>3</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="18">
+        <v>10000</v>
+      </c>
+      <c r="E10" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F10" s="2">
+        <v>10000</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1728</v>
+      </c>
+      <c r="H10" s="2">
+        <v>125</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2">
+        <v>10000</v>
+      </c>
+      <c r="K10" s="19">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="26">
+        <v>4</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="18">
+        <v>10000</v>
+      </c>
+      <c r="E11" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F11" s="2">
+        <v>10000</v>
+      </c>
+      <c r="G11" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="I11" s="2">
+        <v>216</v>
+      </c>
+      <c r="J11" s="2">
+        <v>10000</v>
+      </c>
+      <c r="K11" s="19">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="26">
+        <v>5</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="18">
+        <v>10000</v>
+      </c>
+      <c r="E12" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F12" s="2">
+        <v>10000</v>
+      </c>
+      <c r="G12" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H12" s="2">
+        <v>10000</v>
+      </c>
+      <c r="I12" s="2">
+        <v>2197</v>
+      </c>
+      <c r="J12" s="2">
+        <v>64</v>
+      </c>
+      <c r="K12" s="19">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="26">
+        <v>6</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="18">
+        <v>10000</v>
+      </c>
+      <c r="E13" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F13" s="2">
+        <v>10000</v>
+      </c>
+      <c r="G13" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H13" s="2">
+        <v>10000</v>
+      </c>
+      <c r="I13" s="2">
+        <v>10000</v>
+      </c>
+      <c r="J13" s="2">
+        <v>512</v>
+      </c>
+      <c r="K13" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="26">
+        <v>7</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="20">
+        <v>10000</v>
+      </c>
+      <c r="E14" s="21">
+        <v>10000</v>
+      </c>
+      <c r="F14" s="21">
+        <v>10000</v>
+      </c>
+      <c r="G14" s="21">
+        <v>10000</v>
+      </c>
+      <c r="H14" s="21">
+        <v>10000</v>
+      </c>
+      <c r="I14" s="21">
+        <v>10000</v>
+      </c>
+      <c r="J14" s="21">
+        <v>10000</v>
+      </c>
+      <c r="K14" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D15" s="30">
+        <v>0</v>
+      </c>
+      <c r="E15" s="29">
+        <v>0</v>
+      </c>
+      <c r="F15" s="29">
+        <v>0</v>
+      </c>
+      <c r="G15" s="29">
+        <v>0</v>
+      </c>
+      <c r="H15" s="29">
+        <v>1</v>
+      </c>
+      <c r="I15" s="29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f>D7</f>
+        <v>1728</v>
+      </c>
+      <c r="E16">
+        <f>D16+E7</f>
+        <v>2457</v>
+      </c>
+      <c r="F16">
+        <f>F7+D16</f>
+        <v>2071</v>
+      </c>
+      <c r="G16">
+        <f>G7+D16</f>
+        <v>1736</v>
+      </c>
+      <c r="H16">
+        <v>1728</v>
+      </c>
+      <c r="I16">
+        <v>1952</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17">
+        <v>4</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="J17">
+        <v>6</v>
+      </c>
+      <c r="K17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <f>H8+D16</f>
+        <v>1728</v>
+      </c>
+      <c r="I18">
+        <f>I10+F16</f>
+        <v>2072</v>
+      </c>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <f>H9+E16</f>
+        <v>2484</v>
+      </c>
+      <c r="I19">
+        <f>I11+G16</f>
+        <v>1952</v>
+      </c>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <f>H10+F16</f>
+        <v>2196</v>
+      </c>
+      <c r="I20">
+        <f>I12+H16</f>
+        <v>3925</v>
+      </c>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <f>H11+G16</f>
+        <v>2736</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>